<commit_message>
update the documentation of bytecode command
</commit_message>
<xml_diff>
--- a/blockly/Skoolbot/Bytecode_command.xlsx
+++ b/blockly/Skoolbot/Bytecode_command.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingyuan/Desktop/blockly/blockly/Skoolbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ADAA24-AAE4-454C-A6F2-076C3C39B704}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32285BD-A844-0446-9DA5-FB109F611C93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,27 +162,18 @@
     <t>logic</t>
   </si>
   <si>
-    <t>logic_boolean</t>
-  </si>
-  <si>
     <t>logic_boolean_boolean</t>
   </si>
   <si>
     <t>TRUE, FALSE</t>
   </si>
   <si>
-    <t>logic_null</t>
-  </si>
-  <si>
     <t>logic_null_null</t>
   </si>
   <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>variables_get</t>
-  </si>
-  <si>
     <t>variables</t>
   </si>
   <si>
@@ -204,22 +195,31 @@
     <t>controls</t>
   </si>
   <si>
-    <t>controls_if</t>
-  </si>
-  <si>
     <t>controls_statement_if</t>
   </si>
   <si>
-    <t>controls_else</t>
-  </si>
-  <si>
     <t>controls_statement_else</t>
   </si>
   <si>
-    <t>IF, JUMPZ L0_n(n = 0, 1, 2, 3 ...)</t>
-  </si>
-  <si>
-    <t>ELSE, JUMP L1_n(n = 0, 1, 2, 3 ...)</t>
+    <t>JUMPZ L0_n(n = 0, 1, 2, 3 ...)</t>
+  </si>
+  <si>
+    <t>JUMP L1_n(n = 0, 1, 2, 3 ...)</t>
+  </si>
+  <si>
+    <t>controls_if(if)</t>
+  </si>
+  <si>
+    <t>controls_else(else)</t>
+  </si>
+  <si>
+    <t>variables_get(variable assignment)</t>
+  </si>
+  <si>
+    <t>logic_boolean(true, false)</t>
+  </si>
+  <si>
+    <t>logic_null(null)</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCCD21F-60C4-344A-A1E7-34113DE85D82}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="157" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,13 +809,13 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -823,69 +823,69 @@
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
while control generator update
</commit_message>
<xml_diff>
--- a/blockly/Skoolbot/Bytecode_command.xlsx
+++ b/blockly/Skoolbot/Bytecode_command.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingyuan/Desktop/blockly/blockly/Skoolbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32285BD-A844-0446-9DA5-FB109F611C93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5CD2E3-AC80-354D-AB44-CC9FDB179225}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,6 +237,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -262,11 +270,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,15 +592,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCCD21F-60C4-344A-A1E7-34113DE85D82}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="157" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="69.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -604,7 +613,7 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -618,7 +627,7 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -632,7 +641,7 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -646,7 +655,7 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -660,7 +669,7 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -674,7 +683,7 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -688,7 +697,7 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -702,7 +711,7 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -716,7 +725,7 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -730,7 +739,7 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -744,7 +753,7 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -758,7 +767,7 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -772,7 +781,7 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -786,7 +795,7 @@
       <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -800,7 +809,7 @@
       <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -814,7 +823,7 @@
       <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -828,7 +837,7 @@
       <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -842,7 +851,7 @@
       <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -856,7 +865,7 @@
       <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -870,7 +879,7 @@
       <c r="C20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -884,7 +893,7 @@
       <c r="C21" t="s">
         <v>55</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update simple test case for each block
</commit_message>
<xml_diff>
--- a/blockly/Skoolbot/Bytecode_command.xlsx
+++ b/blockly/Skoolbot/Bytecode_command.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingyuan/Desktop/blockly/blockly/Skoolbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5CD2E3-AC80-354D-AB44-CC9FDB179225}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0D1922-88A6-D346-BB70-0B75F350BBEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>Block Name</t>
   </si>
@@ -42,15 +42,6 @@
     <t>logic_compare (=, ≠, &lt;, ≤,  &gt;, ≥)</t>
   </si>
   <si>
-    <t>math_single (sqrt, abs, -, ln, log10, e^, 10^)</t>
-  </si>
-  <si>
-    <t>math_trig (sin, cos, tan, asin, acos, atan)</t>
-  </si>
-  <si>
-    <t>math_number_property (Even/Odd/prime/whole/positive/negative/divisible by)</t>
-  </si>
-  <si>
     <t>math_number</t>
   </si>
   <si>
@@ -63,12 +54,6 @@
     <t>math_random_int (range (num1-num2))</t>
   </si>
   <si>
-    <t>math_random_float (random faction)</t>
-  </si>
-  <si>
-    <t>math_map (var, range1(num1-num2) to range2(num3-num4))</t>
-  </si>
-  <si>
     <t>math_arithmetic_operator</t>
   </si>
   <si>
@@ -93,21 +78,12 @@
     <t>math_number_operator_modulo</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>math_number_operator_constrain</t>
   </si>
   <si>
     <t>math_number_function_randomInt</t>
   </si>
   <si>
-    <t>math_number_function_randomFloat</t>
-  </si>
-  <si>
-    <t>math_number_constant_constant</t>
-  </si>
-  <si>
     <t>math_number_number</t>
   </si>
   <si>
@@ -120,30 +96,6 @@
     <t>add, sub, mul, div, pow</t>
   </si>
   <si>
-    <t>math_round (round/round up/down)</t>
-  </si>
-  <si>
-    <t>round, roundup, rounddown</t>
-  </si>
-  <si>
-    <t>sqrt, abs, neg, ln, log10, exp, pow10</t>
-  </si>
-  <si>
-    <t>sin, cos, tan, asin, acos, atan</t>
-  </si>
-  <si>
-    <t>math_on_list(sum, min, max, average, median, modes, standard deviation, random item)</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
-    <t>math_constant (PI, e, INFINITY)</t>
-  </si>
-  <si>
-    <t>isEven, isOdd, isPrime, isWhole, isPositive, isNegative, isDivisibleBy</t>
-  </si>
-  <si>
     <t>remainder</t>
   </si>
   <si>
@@ -153,9 +105,6 @@
     <t>randomInt</t>
   </si>
   <si>
-    <t>randomFloat</t>
-  </si>
-  <si>
     <t>math</t>
   </si>
   <si>
@@ -220,6 +169,45 @@
   </si>
   <si>
     <t>logic_null(null)</t>
+  </si>
+  <si>
+    <t>semantic or structure</t>
+  </si>
+  <si>
+    <t>math_single (abs, -)</t>
+  </si>
+  <si>
+    <t>abs, neg</t>
+  </si>
+  <si>
+    <t>math_number_property (Even/Odd/positive/negative/divisible by)</t>
+  </si>
+  <si>
+    <t>isEven, isOdd, isPositive, isNegative, isDivisibleBy</t>
+  </si>
+  <si>
+    <t>logic_negate</t>
+  </si>
+  <si>
+    <t>logic_boolean_operator_logicNegate</t>
+  </si>
+  <si>
+    <t>negate</t>
+  </si>
+  <si>
+    <t>number 10</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; &lt;arg_2&gt; add</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; neg</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; isEven / &lt;arg_1&gt; &lt;arg_2&gt; isDivisibleBy</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; &lt;arg_2&gt; remainder</t>
   </si>
 </sst>
 </file>
@@ -590,311 +578,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCCD21F-60C4-344A-A1E7-34113DE85D82}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="69.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix generator for test
</commit_message>
<xml_diff>
--- a/blockly/Skoolbot/Bytecode_command.xlsx
+++ b/blockly/Skoolbot/Bytecode_command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingyuan/Desktop/blockly/blockly/Skoolbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0D1922-88A6-D346-BB70-0B75F350BBEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972EE618-E370-EB4A-9DDD-F0F3D7031956}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>Block Name</t>
   </si>
@@ -208,6 +208,30 @@
   </si>
   <si>
     <t>&lt;arg_1&gt; &lt;arg_2&gt; remainder</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; &lt;arg_2&gt; &lt;arg_3&gt; constrain</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; &lt;arg_2&gt; randomInt</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt; &lt;arg_2&gt; cmpe</t>
+  </si>
+  <si>
+    <t>&lt;boolean&gt; negate</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>get &lt;variable name&gt;</t>
+  </si>
+  <si>
+    <t>set &lt;variable name&gt;</t>
+  </si>
+  <si>
+    <t>boolean TRUE/boolean FALSE</t>
   </si>
 </sst>
 </file>
@@ -580,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCCD21F-60C4-344A-A1E7-34113DE85D82}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,6 +731,9 @@
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -721,6 +748,9 @@
       <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -735,6 +765,9 @@
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -749,6 +782,9 @@
       <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -763,6 +799,9 @@
       <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -777,6 +816,9 @@
       <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -791,6 +833,9 @@
       <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -804,6 +849,9 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix repeat and while test cases
</commit_message>
<xml_diff>
--- a/blockly/Skoolbot/Bytecode_command.xlsx
+++ b/blockly/Skoolbot/Bytecode_command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingyuan/Desktop/blockly/blockly/Skoolbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972EE618-E370-EB4A-9DDD-F0F3D7031956}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FC8576-7D6A-B845-9FB1-D7DAD1994056}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Block Name</t>
   </si>
@@ -144,24 +144,6 @@
     <t>controls</t>
   </si>
   <si>
-    <t>controls_statement_if</t>
-  </si>
-  <si>
-    <t>controls_statement_else</t>
-  </si>
-  <si>
-    <t>JUMPZ L0_n(n = 0, 1, 2, 3 ...)</t>
-  </si>
-  <si>
-    <t>JUMP L1_n(n = 0, 1, 2, 3 ...)</t>
-  </si>
-  <si>
-    <t>controls_if(if)</t>
-  </si>
-  <si>
-    <t>controls_else(else)</t>
-  </si>
-  <si>
     <t>variables_get(variable assignment)</t>
   </si>
   <si>
@@ -171,9 +153,6 @@
     <t>logic_null(null)</t>
   </si>
   <si>
-    <t>semantic or structure</t>
-  </si>
-  <si>
     <t>math_single (abs, -)</t>
   </si>
   <si>
@@ -198,27 +177,6 @@
     <t>number 10</t>
   </si>
   <si>
-    <t>&lt;arg_1&gt; &lt;arg_2&gt; add</t>
-  </si>
-  <si>
-    <t>&lt;arg_1&gt; neg</t>
-  </si>
-  <si>
-    <t>&lt;arg_1&gt; isEven / &lt;arg_1&gt; &lt;arg_2&gt; isDivisibleBy</t>
-  </si>
-  <si>
-    <t>&lt;arg_1&gt; &lt;arg_2&gt; remainder</t>
-  </si>
-  <si>
-    <t>&lt;arg_1&gt; &lt;arg_2&gt; &lt;arg_3&gt; constrain</t>
-  </si>
-  <si>
-    <t>&lt;arg_1&gt; &lt;arg_2&gt; randomInt</t>
-  </si>
-  <si>
-    <t>&lt;arg_1&gt; &lt;arg_2&gt; cmpe</t>
-  </si>
-  <si>
     <t>&lt;boolean&gt; negate</t>
   </si>
   <si>
@@ -231,24 +189,99 @@
     <t>set &lt;variable name&gt;</t>
   </si>
   <si>
-    <t>boolean TRUE/boolean FALSE</t>
+    <t>controls_while</t>
+  </si>
+  <si>
+    <t>Semantic or Structure</t>
+  </si>
+  <si>
+    <t>boolean TRUE/ boolean FALSE</t>
+  </si>
+  <si>
+    <t>controls_statement_ifelse</t>
+  </si>
+  <si>
+    <t>JUMPZ L0_n(n = 0, 1, 2, 3 ...)    /  JUMP L1_n(n = 0, 1, 2, 3 ...)</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt;
+&lt;arg_2&gt;
+cmpe</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt;
+&lt;arg_2&gt;
+randomInt</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt;
+&lt;arg_2&gt;
+&lt;arg_3&gt;
+constrain</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt;
+&lt;arg_2&gt;
+remainder</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt;
+neg</t>
+  </si>
+  <si>
+    <t>&lt;arg_1&gt;
+&lt;arg_2&gt;
+add</t>
+  </si>
+  <si>
+    <t>case1:
+&lt;arg_1&gt;
+isEven / 
+case2
+&lt;arg_1&gt;
+&lt;arg_2&gt;
+isDivisibleBy</t>
+  </si>
+  <si>
+    <t>&lt;condition&gt;
+JUMPZ L0_n
+&lt;true branch&gt;
+JUMP L1_n
+L0_n
+&lt;false branch&gt;
+L1_n</t>
+  </si>
+  <si>
+    <t>controls_if</t>
+  </si>
+  <si>
+    <t>controls_statement_for</t>
+  </si>
+  <si>
+    <t>&lt;init i&gt;
+L0_n
+&lt;end condition&gt;
+JUMPZ L1_n
+&lt;step increment&gt;
+&lt;statement&gt;
+JUMP L0_n
+L1_n</t>
+  </si>
+  <si>
+    <t>controls_whileUntil</t>
+  </si>
+  <si>
+    <t>controls_statement_whileUntil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -284,10 +317,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,284 +635,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCCD21F-60C4-344A-A1E7-34113DE85D82}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="157" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="69.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
-        <v>46</v>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>47</v>
+      <c r="B4" t="s">
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>49</v>
+      <c r="B5" t="s">
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
-        <v>61</v>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
+      <c r="B10" t="s">
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>51</v>
+      <c r="B11" t="s">
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
+      <c r="B12" t="s">
+        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>43</v>
+      <c r="B13" t="s">
+        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>41</v>
+      <c r="B15" t="s">
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>42</v>
+      <c r="B16" t="s">
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restructure the generator functions
</commit_message>
<xml_diff>
--- a/blockly/Skoolbot/Bytecode_command.xlsx
+++ b/blockly/Skoolbot/Bytecode_command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingyuan/Desktop/blockly/blockly/Skoolbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8137E94C-480E-724C-9236-57F5ADF2DDF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66AF12-4A08-E448-B633-1B0ABF5D9DFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0F423905-75F0-614D-9E46-D2B54CDBB64B}"/>
   </bookViews>
@@ -234,15 +234,6 @@
 add</t>
   </si>
   <si>
-    <t>case1:
-&lt;arg_1&gt;
-isEven / 
-case2
-&lt;arg_1&gt;
-&lt;arg_2&gt;
-isDivisibleBy</t>
-  </si>
-  <si>
     <t>&lt;condition&gt;
 JUMPZ L0_n
 &lt;true branch&gt;
@@ -287,6 +278,15 @@
   </si>
   <si>
     <t>controls_statement_repeat</t>
+  </si>
+  <si>
+    <t>case1:
+&lt;arg_1&gt;
+isEven / 
+case2:
+&lt;arg_1&gt;
+&lt;arg_2&gt;
+isDivisibleBy</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCCD21F-60C4-344A-A1E7-34113DE85D82}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="157" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -660,7 +660,7 @@
   <cols>
     <col min="2" max="2" width="69.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -746,7 +746,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -907,7 +907,7 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>55</v>
@@ -916,7 +916,7 @@
         <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="136" x14ac:dyDescent="0.2">
@@ -927,13 +927,13 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="119" x14ac:dyDescent="0.2">
@@ -941,16 +941,16 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -958,10 +958,10 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
         <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>56</v>

</xml_diff>